<commit_message>
100 downloads xlsx, extracts csv
</commit_message>
<xml_diff>
--- a/documentation-generator/vocab_csv/entities.xlsx
+++ b/documentation-generator/vocab_csv/entities.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="810" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="332">
   <si>
     <t>Term</t>
   </si>
@@ -689,9 +689,15 @@
     <t>ReligiousAssociations</t>
   </si>
   <si>
+    <t>Religious Associations</t>
+  </si>
+  <si>
     <t>DISCUSS TBD</t>
   </si>
   <si>
+    <t>dpv:Organisation</t>
+  </si>
+  <si>
     <t>Organisation</t>
   </si>
   <si>
@@ -705,9 +711,6 @@
   </si>
   <si>
     <t>A consortium established and comprising on industry organisations</t>
-  </si>
-  <si>
-    <t>dpv:Organisation</t>
   </si>
   <si>
     <t>(ADMS controlled vocabulary,http://purl.org/adms)</t>
@@ -10164,12 +10167,18 @@
       <c r="A2" s="36" t="s">
         <v>196</v>
       </c>
-      <c r="B2" s="37"/>
+      <c r="B2" s="37" t="s">
+        <v>197</v>
+      </c>
       <c r="C2" s="13" t="s">
-        <v>197</v>
-      </c>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
+        <v>198</v>
+      </c>
+      <c r="D2" s="37" t="s">
+        <v>199</v>
+      </c>
+      <c r="E2" s="37" t="s">
+        <v>26</v>
+      </c>
       <c r="F2" s="37"/>
       <c r="G2" s="37"/>
       <c r="H2" s="43"/>
@@ -10198,13 +10207,13 @@
     </row>
     <row r="3">
       <c r="A3" s="21" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B3" s="80" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D3" s="21" t="s">
         <v>34</v>
@@ -10246,16 +10255,16 @@
     </row>
     <row r="4">
       <c r="A4" s="21" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B4" s="87" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="D4" s="84" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="E4" s="22" t="s">
         <v>26</v>
@@ -10265,7 +10274,7 @@
       <c r="H4" s="23"/>
       <c r="I4" s="23"/>
       <c r="J4" s="21" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="K4" s="25">
         <v>44594.0</v>
@@ -10298,16 +10307,16 @@
     </row>
     <row r="5">
       <c r="A5" s="21" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B5" s="65" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D5" s="84" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="E5" s="22" t="s">
         <v>26</v>
@@ -10348,16 +10357,16 @@
     </row>
     <row r="6">
       <c r="A6" s="21" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B6" s="87" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D6" s="84" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="E6" s="22" t="s">
         <v>26</v>
@@ -10367,7 +10376,7 @@
       <c r="H6" s="23"/>
       <c r="I6" s="23"/>
       <c r="J6" s="21" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="K6" s="25">
         <v>44594.0</v>
@@ -10400,16 +10409,16 @@
     </row>
     <row r="7">
       <c r="A7" s="21" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B7" s="87" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D7" s="84" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="E7" s="22" t="s">
         <v>26</v>
@@ -10450,16 +10459,16 @@
     </row>
     <row r="8">
       <c r="A8" s="21" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B8" s="87" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D8" s="84" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="E8" s="22" t="s">
         <v>26</v>
@@ -10469,7 +10478,7 @@
       <c r="H8" s="23"/>
       <c r="I8" s="23"/>
       <c r="J8" s="21" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="K8" s="25">
         <v>44594.0</v>
@@ -10502,16 +10511,16 @@
     </row>
     <row r="9">
       <c r="A9" s="21" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B9" s="87" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D9" s="84" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="E9" s="22" t="s">
         <v>26</v>
@@ -10521,7 +10530,7 @@
       <c r="H9" s="23"/>
       <c r="I9" s="23"/>
       <c r="J9" s="21" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="K9" s="25">
         <v>44594.0</v>
@@ -10554,16 +10563,16 @@
     </row>
     <row r="10">
       <c r="A10" s="48" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B10" s="48" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C10" s="48" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="D10" s="49" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="E10" s="22" t="s">
         <v>26</v>
@@ -10573,7 +10582,7 @@
       <c r="H10" s="23"/>
       <c r="I10" s="23"/>
       <c r="J10" s="57" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="K10" s="52">
         <v>44643.0</v>
@@ -10585,10 +10594,10 @@
         <v>154</v>
       </c>
       <c r="N10" s="48" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="O10" s="89" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="P10" s="28"/>
       <c r="Q10" s="28"/>
@@ -10606,13 +10615,13 @@
     </row>
     <row r="11">
       <c r="A11" s="48" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B11" s="48" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C11" s="49" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="D11" s="22" t="s">
         <v>25</v>
@@ -10633,10 +10642,10 @@
         <v>19</v>
       </c>
       <c r="N11" s="48" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="O11" s="89" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="P11" s="28"/>
       <c r="Q11" s="28"/>
@@ -10654,10 +10663,10 @@
     </row>
     <row r="12">
       <c r="A12" s="90" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B12" s="90" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C12" s="14"/>
       <c r="D12" s="13" t="s">
@@ -10694,10 +10703,10 @@
     </row>
     <row r="13">
       <c r="A13" s="90" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B13" s="90" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C13" s="14"/>
       <c r="D13" s="13" t="s">
@@ -10734,10 +10743,10 @@
     </row>
     <row r="14">
       <c r="A14" s="90" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B14" s="90" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C14" s="14"/>
       <c r="D14" s="13" t="s">
@@ -10774,10 +10783,10 @@
     </row>
     <row r="15">
       <c r="A15" s="90" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B15" s="90" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C15" s="14"/>
       <c r="D15" s="13" t="s">
@@ -10814,10 +10823,10 @@
     </row>
     <row r="16">
       <c r="A16" s="90" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B16" s="90" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C16" s="14"/>
       <c r="D16" s="13" t="s">
@@ -10942,13 +10951,13 @@
     </row>
     <row r="2">
       <c r="A2" s="80" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B2" s="80" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C2" s="80" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D2" s="80" t="s">
         <v>17</v>
@@ -10995,13 +11004,13 @@
     </row>
     <row r="3">
       <c r="A3" s="13" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>17</v>
@@ -11037,13 +11046,13 @@
     </row>
     <row r="4">
       <c r="A4" s="13" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>25</v>
@@ -11066,10 +11075,10 @@
         <v>19</v>
       </c>
       <c r="N4" s="13" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="O4" s="45" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="P4" s="14"/>
       <c r="Q4" s="14"/>
@@ -11178,16 +11187,16 @@
     </row>
     <row r="2">
       <c r="A2" s="60" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B2" s="60" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C2" s="91" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D2" s="92" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="E2" s="93" t="s">
         <v>26</v>
@@ -11196,10 +11205,10 @@
       <c r="G2" s="28"/>
       <c r="H2" s="23"/>
       <c r="I2" s="60" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="J2" s="94" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="K2" s="82">
         <v>43560.0</v>
@@ -11232,16 +11241,16 @@
     </row>
     <row r="3">
       <c r="A3" s="59" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B3" s="60" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C3" s="59" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="D3" s="65" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E3" s="93" t="s">
         <v>26</v>
@@ -11250,7 +11259,7 @@
       <c r="G3" s="23"/>
       <c r="H3" s="23"/>
       <c r="I3" s="97" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="J3" s="23"/>
       <c r="K3" s="25">
@@ -11260,7 +11269,7 @@
         <v>44734.0</v>
       </c>
       <c r="M3" s="65" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="N3" s="59" t="s">
         <v>20</v>
@@ -11284,16 +11293,16 @@
     </row>
     <row r="4">
       <c r="A4" s="13" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E4" s="93" t="s">
         <v>26</v>
@@ -11311,10 +11320,10 @@
         <v>19</v>
       </c>
       <c r="N4" s="37" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="O4" s="45" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="P4" s="14"/>
       <c r="Q4" s="14"/>
@@ -11332,16 +11341,16 @@
     </row>
     <row r="5">
       <c r="A5" s="59" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B5" s="60" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C5" s="59" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D5" s="59" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E5" s="93" t="s">
         <v>26</v>
@@ -11350,7 +11359,7 @@
       <c r="G5" s="23"/>
       <c r="H5" s="23"/>
       <c r="I5" s="99" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="J5" s="59"/>
       <c r="K5" s="25">
@@ -11382,16 +11391,16 @@
     </row>
     <row r="6">
       <c r="A6" s="13" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E6" s="93" t="s">
         <v>26</v>
@@ -11409,10 +11418,10 @@
         <v>19</v>
       </c>
       <c r="N6" s="13" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="O6" s="45" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="P6" s="14"/>
       <c r="Q6" s="14"/>
@@ -11430,16 +11439,16 @@
     </row>
     <row r="7">
       <c r="A7" s="13" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E7" s="93" t="s">
         <v>26</v>
@@ -11457,10 +11466,10 @@
         <v>19</v>
       </c>
       <c r="N7" s="13" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="O7" s="45" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="P7" s="14"/>
       <c r="Q7" s="14"/>
@@ -11478,16 +11487,16 @@
     </row>
     <row r="8">
       <c r="A8" s="13" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E8" s="93" t="s">
         <v>26</v>
@@ -11505,10 +11514,10 @@
         <v>19</v>
       </c>
       <c r="N8" s="13" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="O8" s="45" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="P8" s="14"/>
       <c r="Q8" s="14"/>
@@ -11526,16 +11535,16 @@
     </row>
     <row r="9">
       <c r="A9" s="13" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E9" s="93" t="s">
         <v>26</v>
@@ -11553,10 +11562,10 @@
         <v>19</v>
       </c>
       <c r="N9" s="13" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="O9" s="45" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="P9" s="14"/>
       <c r="Q9" s="14"/>
@@ -11574,16 +11583,16 @@
     </row>
     <row r="10">
       <c r="A10" s="13" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E10" s="93" t="s">
         <v>26</v>
@@ -11601,10 +11610,10 @@
         <v>19</v>
       </c>
       <c r="N10" s="13" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="O10" s="45" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="P10" s="14"/>
       <c r="Q10" s="14"/>
@@ -11622,16 +11631,16 @@
     </row>
     <row r="11">
       <c r="A11" s="13" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E11" s="93" t="s">
         <v>26</v>
@@ -11649,10 +11658,10 @@
         <v>19</v>
       </c>
       <c r="N11" s="13" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="O11" s="45" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="P11" s="14"/>
       <c r="Q11" s="14"/>
@@ -11670,16 +11679,16 @@
     </row>
     <row r="12">
       <c r="A12" s="13" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E12" s="93" t="s">
         <v>26</v>
@@ -11697,10 +11706,10 @@
         <v>19</v>
       </c>
       <c r="N12" s="13" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="O12" s="45" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="P12" s="14"/>
       <c r="Q12" s="14"/>
@@ -11718,16 +11727,16 @@
     </row>
     <row r="13">
       <c r="A13" s="13" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="D13" s="100" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E13" s="93" t="s">
         <v>26</v>
@@ -11736,7 +11745,7 @@
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
       <c r="I13" s="13" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="J13" s="14"/>
       <c r="K13" s="15">
@@ -11747,10 +11756,10 @@
         <v>19</v>
       </c>
       <c r="N13" s="13" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="O13" s="45" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="P13" s="14"/>
       <c r="Q13" s="14"/>
@@ -11768,16 +11777,16 @@
     </row>
     <row r="14">
       <c r="A14" s="13" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E14" s="93" t="s">
         <v>26</v>
@@ -11795,10 +11804,10 @@
         <v>19</v>
       </c>
       <c r="N14" s="13" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="O14" s="45" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="P14" s="14"/>
       <c r="Q14" s="14"/>
@@ -11816,16 +11825,16 @@
     </row>
     <row r="15">
       <c r="A15" s="13" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E15" s="93" t="s">
         <v>26</v>
@@ -11843,10 +11852,10 @@
         <v>19</v>
       </c>
       <c r="N15" s="13" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="O15" s="45" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="P15" s="14"/>
       <c r="Q15" s="14"/>
@@ -11864,16 +11873,16 @@
     </row>
     <row r="16">
       <c r="A16" s="13" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="E16" s="93" t="s">
         <v>26</v>
@@ -11891,10 +11900,10 @@
         <v>19</v>
       </c>
       <c r="N16" s="13" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="O16" s="45" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="P16" s="14"/>
       <c r="Q16" s="14"/>
@@ -11912,16 +11921,16 @@
     </row>
     <row r="17">
       <c r="A17" s="13" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E17" s="93" t="s">
         <v>26</v>
@@ -11939,10 +11948,10 @@
         <v>19</v>
       </c>
       <c r="N17" s="13" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="O17" s="45" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="P17" s="14"/>
       <c r="Q17" s="14"/>
@@ -11960,16 +11969,16 @@
     </row>
     <row r="18">
       <c r="A18" s="13" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E18" s="93" t="s">
         <v>26</v>
@@ -11987,10 +11996,10 @@
         <v>19</v>
       </c>
       <c r="N18" s="13" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="O18" s="45" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="P18" s="14"/>
       <c r="Q18" s="14"/>
@@ -12008,16 +12017,16 @@
     </row>
     <row r="19">
       <c r="A19" s="13" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E19" s="93" t="s">
         <v>26</v>
@@ -12035,10 +12044,10 @@
         <v>19</v>
       </c>
       <c r="N19" s="13" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="O19" s="45" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="P19" s="14"/>
       <c r="Q19" s="14"/>
@@ -12056,16 +12065,16 @@
     </row>
     <row r="20">
       <c r="A20" s="13" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E20" s="93" t="s">
         <v>26</v>
@@ -12074,7 +12083,7 @@
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
       <c r="I20" s="13" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="J20" s="14"/>
       <c r="K20" s="15">
@@ -12085,10 +12094,10 @@
         <v>19</v>
       </c>
       <c r="N20" s="13" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="O20" s="45" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="P20" s="14"/>
       <c r="Q20" s="14"/>
@@ -12106,16 +12115,16 @@
     </row>
     <row r="21">
       <c r="A21" s="13" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="E21" s="93" t="s">
         <v>26</v>
@@ -12133,10 +12142,10 @@
         <v>19</v>
       </c>
       <c r="N21" s="13" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="O21" s="45" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="P21" s="14"/>
       <c r="Q21" s="14"/>
@@ -12154,16 +12163,16 @@
     </row>
     <row r="22">
       <c r="A22" s="13" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E22" s="93" t="s">
         <v>26</v>
@@ -12181,10 +12190,10 @@
         <v>19</v>
       </c>
       <c r="N22" s="13" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="O22" s="45" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="P22" s="14"/>
       <c r="Q22" s="14"/>
@@ -12202,16 +12211,16 @@
     </row>
     <row r="23">
       <c r="A23" s="13" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="E23" s="93" t="s">
         <v>26</v>
@@ -12229,10 +12238,10 @@
         <v>19</v>
       </c>
       <c r="N23" s="13" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="O23" s="45" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="P23" s="14"/>
       <c r="Q23" s="14"/>
@@ -12250,16 +12259,16 @@
     </row>
     <row r="24">
       <c r="A24" s="13" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="E24" s="93" t="s">
         <v>26</v>
@@ -12277,10 +12286,10 @@
         <v>19</v>
       </c>
       <c r="N24" s="13" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="O24" s="45" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="P24" s="14"/>
       <c r="Q24" s="14"/>
@@ -12298,16 +12307,16 @@
     </row>
     <row r="25">
       <c r="A25" s="13" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="E25" s="93" t="s">
         <v>26</v>
@@ -12325,10 +12334,10 @@
         <v>19</v>
       </c>
       <c r="N25" s="13" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="O25" s="45" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="P25" s="14"/>
       <c r="Q25" s="14"/>
@@ -12346,16 +12355,16 @@
     </row>
     <row r="26">
       <c r="A26" s="13" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E26" s="93" t="s">
         <v>26</v>
@@ -12373,10 +12382,10 @@
         <v>19</v>
       </c>
       <c r="N26" s="13" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="O26" s="45" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="P26" s="14"/>
       <c r="Q26" s="14"/>
@@ -12394,16 +12403,16 @@
     </row>
     <row r="27">
       <c r="A27" s="13" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E27" s="93" t="s">
         <v>26</v>
@@ -12421,10 +12430,10 @@
         <v>19</v>
       </c>
       <c r="N27" s="13" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="O27" s="45" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="P27" s="14"/>
       <c r="Q27" s="14"/>

</xml_diff>

<commit_message>
200 handles taxonomy topconcept
</commit_message>
<xml_diff>
--- a/documentation-generator/vocab_csv/entities.xlsx
+++ b/documentation-generator/vocab_csv/entities.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="330">
   <si>
     <t>Term</t>
   </si>
@@ -898,9 +898,6 @@
     <t>The legality of age defining a child varies by jurisdiction. In addition, 'child' is distinct from a 'minor'. For example, the legal age for consumption of alcohol can be 21, which makes a person of age 20 a 'minor' in this context. In other cases, 'minor' and 'child' are used interchangeably to refer to a person below some legally defined age.</t>
   </si>
   <si>
-    <t>changed</t>
-  </si>
-  <si>
     <t>Adult</t>
   </si>
   <si>
@@ -1004,9 +1001,6 @@
   </si>
   <si>
     <t>Data subjects that apply for jobs or employments</t>
-  </si>
-  <si>
-    <t>dpv:Applicant</t>
   </si>
   <si>
     <t>Visitor</t>
@@ -1115,7 +1109,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
   </numFmts>
-  <fonts count="35">
+  <fonts count="34">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -1281,10 +1275,6 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font>
-      <color rgb="FF0000FF"/>
-      <name val="&quot;Arial&quot;"/>
-    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1382,7 +1372,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="100">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1676,9 +1666,6 @@
     </xf>
     <xf borderId="1" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="34" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -11249,11 +11236,9 @@
       <c r="C3" s="59" t="s">
         <v>259</v>
       </c>
-      <c r="D3" s="65" t="s">
+      <c r="D3" s="14"/>
+      <c r="E3" s="65" t="s">
         <v>260</v>
-      </c>
-      <c r="E3" s="93" t="s">
-        <v>26</v>
       </c>
       <c r="F3" s="23"/>
       <c r="G3" s="23"/>
@@ -11269,7 +11254,7 @@
         <v>44734.0</v>
       </c>
       <c r="M3" s="65" t="s">
-        <v>262</v>
+        <v>19</v>
       </c>
       <c r="N3" s="59" t="s">
         <v>20</v>
@@ -11293,19 +11278,17 @@
     </row>
     <row r="4">
       <c r="A4" s="13" t="s">
+        <v>262</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>262</v>
+      </c>
+      <c r="C4" s="13" t="s">
         <v>263</v>
       </c>
-      <c r="B4" s="13" t="s">
-        <v>263</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>264</v>
-      </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="14"/>
+      <c r="E4" s="65" t="s">
         <v>260</v>
-      </c>
-      <c r="E4" s="93" t="s">
-        <v>26</v>
       </c>
       <c r="F4" s="14"/>
       <c r="G4" s="14"/>
@@ -11320,10 +11303,10 @@
         <v>19</v>
       </c>
       <c r="N4" s="37" t="s">
+        <v>264</v>
+      </c>
+      <c r="O4" s="45" t="s">
         <v>265</v>
-      </c>
-      <c r="O4" s="45" t="s">
-        <v>266</v>
       </c>
       <c r="P4" s="14"/>
       <c r="Q4" s="14"/>
@@ -11341,25 +11324,23 @@
     </row>
     <row r="5">
       <c r="A5" s="59" t="s">
+        <v>266</v>
+      </c>
+      <c r="B5" s="60" t="s">
         <v>267</v>
       </c>
-      <c r="B5" s="60" t="s">
+      <c r="C5" s="59" t="s">
         <v>268</v>
       </c>
-      <c r="C5" s="59" t="s">
-        <v>269</v>
-      </c>
-      <c r="D5" s="59" t="s">
+      <c r="D5" s="14"/>
+      <c r="E5" s="65" t="s">
         <v>260</v>
-      </c>
-      <c r="E5" s="93" t="s">
-        <v>26</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="23"/>
       <c r="H5" s="23"/>
       <c r="I5" s="99" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="J5" s="59"/>
       <c r="K5" s="25">
@@ -11391,19 +11372,17 @@
     </row>
     <row r="6">
       <c r="A6" s="13" t="s">
+        <v>270</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>270</v>
+      </c>
+      <c r="C6" s="13" t="s">
         <v>271</v>
       </c>
-      <c r="B6" s="13" t="s">
-        <v>271</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>272</v>
-      </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="14"/>
+      <c r="E6" s="65" t="s">
         <v>260</v>
-      </c>
-      <c r="E6" s="93" t="s">
-        <v>26</v>
       </c>
       <c r="F6" s="14"/>
       <c r="G6" s="14"/>
@@ -11418,10 +11397,10 @@
         <v>19</v>
       </c>
       <c r="N6" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="O6" s="45" t="s">
         <v>273</v>
-      </c>
-      <c r="O6" s="45" t="s">
-        <v>274</v>
       </c>
       <c r="P6" s="14"/>
       <c r="Q6" s="14"/>
@@ -11439,19 +11418,17 @@
     </row>
     <row r="7">
       <c r="A7" s="13" t="s">
+        <v>274</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>274</v>
+      </c>
+      <c r="C7" s="13" t="s">
         <v>275</v>
       </c>
-      <c r="B7" s="13" t="s">
-        <v>275</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>276</v>
-      </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="14"/>
+      <c r="E7" s="65" t="s">
         <v>260</v>
-      </c>
-      <c r="E7" s="93" t="s">
-        <v>26</v>
       </c>
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
@@ -11466,10 +11443,10 @@
         <v>19</v>
       </c>
       <c r="N7" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="O7" s="45" t="s">
         <v>273</v>
-      </c>
-      <c r="O7" s="45" t="s">
-        <v>274</v>
       </c>
       <c r="P7" s="14"/>
       <c r="Q7" s="14"/>
@@ -11487,19 +11464,17 @@
     </row>
     <row r="8">
       <c r="A8" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="C8" s="13" t="s">
         <v>277</v>
       </c>
-      <c r="B8" s="13" t="s">
-        <v>277</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>278</v>
-      </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="14"/>
+      <c r="E8" s="65" t="s">
         <v>260</v>
-      </c>
-      <c r="E8" s="93" t="s">
-        <v>26</v>
       </c>
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
@@ -11514,10 +11489,10 @@
         <v>19</v>
       </c>
       <c r="N8" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="O8" s="45" t="s">
         <v>273</v>
-      </c>
-      <c r="O8" s="45" t="s">
-        <v>274</v>
       </c>
       <c r="P8" s="14"/>
       <c r="Q8" s="14"/>
@@ -11535,19 +11510,17 @@
     </row>
     <row r="9">
       <c r="A9" s="13" t="s">
+        <v>278</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>278</v>
+      </c>
+      <c r="C9" s="13" t="s">
         <v>279</v>
       </c>
-      <c r="B9" s="13" t="s">
-        <v>279</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>280</v>
-      </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="14"/>
+      <c r="E9" s="65" t="s">
         <v>260</v>
-      </c>
-      <c r="E9" s="93" t="s">
-        <v>26</v>
       </c>
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
@@ -11562,10 +11535,10 @@
         <v>19</v>
       </c>
       <c r="N9" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="O9" s="45" t="s">
         <v>273</v>
-      </c>
-      <c r="O9" s="45" t="s">
-        <v>274</v>
       </c>
       <c r="P9" s="14"/>
       <c r="Q9" s="14"/>
@@ -11583,19 +11556,17 @@
     </row>
     <row r="10">
       <c r="A10" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="B10" s="13" t="s">
         <v>281</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="C10" s="13" t="s">
         <v>282</v>
       </c>
-      <c r="C10" s="13" t="s">
-        <v>283</v>
-      </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="14"/>
+      <c r="E10" s="65" t="s">
         <v>260</v>
-      </c>
-      <c r="E10" s="93" t="s">
-        <v>26</v>
       </c>
       <c r="F10" s="14"/>
       <c r="G10" s="14"/>
@@ -11610,10 +11581,10 @@
         <v>19</v>
       </c>
       <c r="N10" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="O10" s="45" t="s">
         <v>273</v>
-      </c>
-      <c r="O10" s="45" t="s">
-        <v>274</v>
       </c>
       <c r="P10" s="14"/>
       <c r="Q10" s="14"/>
@@ -11631,19 +11602,17 @@
     </row>
     <row r="11">
       <c r="A11" s="13" t="s">
+        <v>283</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>283</v>
+      </c>
+      <c r="C11" s="13" t="s">
         <v>284</v>
       </c>
-      <c r="B11" s="13" t="s">
-        <v>284</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>285</v>
-      </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="14"/>
+      <c r="E11" s="65" t="s">
         <v>260</v>
-      </c>
-      <c r="E11" s="93" t="s">
-        <v>26</v>
       </c>
       <c r="F11" s="14"/>
       <c r="G11" s="14"/>
@@ -11658,10 +11627,10 @@
         <v>19</v>
       </c>
       <c r="N11" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="O11" s="45" t="s">
         <v>273</v>
-      </c>
-      <c r="O11" s="45" t="s">
-        <v>274</v>
       </c>
       <c r="P11" s="14"/>
       <c r="Q11" s="14"/>
@@ -11679,19 +11648,17 @@
     </row>
     <row r="12">
       <c r="A12" s="13" t="s">
+        <v>285</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>285</v>
+      </c>
+      <c r="C12" s="13" t="s">
         <v>286</v>
       </c>
-      <c r="B12" s="13" t="s">
-        <v>286</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>287</v>
-      </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="14"/>
+      <c r="E12" s="65" t="s">
         <v>260</v>
-      </c>
-      <c r="E12" s="93" t="s">
-        <v>26</v>
       </c>
       <c r="F12" s="14"/>
       <c r="G12" s="14"/>
@@ -11706,10 +11673,10 @@
         <v>19</v>
       </c>
       <c r="N12" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="O12" s="45" t="s">
         <v>273</v>
-      </c>
-      <c r="O12" s="45" t="s">
-        <v>274</v>
       </c>
       <c r="P12" s="14"/>
       <c r="Q12" s="14"/>
@@ -11727,25 +11694,23 @@
     </row>
     <row r="13">
       <c r="A13" s="13" t="s">
+        <v>287</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>287</v>
+      </c>
+      <c r="C13" s="13" t="s">
         <v>288</v>
       </c>
-      <c r="B13" s="13" t="s">
-        <v>288</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>289</v>
-      </c>
-      <c r="D13" s="100" t="s">
+      <c r="D13" s="14"/>
+      <c r="E13" s="65" t="s">
         <v>260</v>
-      </c>
-      <c r="E13" s="93" t="s">
-        <v>26</v>
       </c>
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
       <c r="I13" s="13" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="J13" s="14"/>
       <c r="K13" s="15">
@@ -11756,10 +11721,10 @@
         <v>19</v>
       </c>
       <c r="N13" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="O13" s="45" t="s">
         <v>273</v>
-      </c>
-      <c r="O13" s="45" t="s">
-        <v>274</v>
       </c>
       <c r="P13" s="14"/>
       <c r="Q13" s="14"/>
@@ -11777,19 +11742,17 @@
     </row>
     <row r="14">
       <c r="A14" s="13" t="s">
+        <v>290</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>290</v>
+      </c>
+      <c r="C14" s="13" t="s">
         <v>291</v>
       </c>
-      <c r="B14" s="13" t="s">
-        <v>291</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>292</v>
-      </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="14"/>
+      <c r="E14" s="65" t="s">
         <v>260</v>
-      </c>
-      <c r="E14" s="93" t="s">
-        <v>26</v>
       </c>
       <c r="F14" s="14"/>
       <c r="G14" s="14"/>
@@ -11804,10 +11767,10 @@
         <v>19</v>
       </c>
       <c r="N14" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="O14" s="45" t="s">
         <v>273</v>
-      </c>
-      <c r="O14" s="45" t="s">
-        <v>274</v>
       </c>
       <c r="P14" s="14"/>
       <c r="Q14" s="14"/>
@@ -11825,19 +11788,17 @@
     </row>
     <row r="15">
       <c r="A15" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="C15" s="13" t="s">
         <v>293</v>
       </c>
-      <c r="B15" s="13" t="s">
-        <v>293</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>294</v>
-      </c>
-      <c r="D15" s="13" t="s">
+      <c r="D15" s="14"/>
+      <c r="E15" s="65" t="s">
         <v>260</v>
-      </c>
-      <c r="E15" s="93" t="s">
-        <v>26</v>
       </c>
       <c r="F15" s="14"/>
       <c r="G15" s="14"/>
@@ -11852,10 +11813,10 @@
         <v>19</v>
       </c>
       <c r="N15" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="O15" s="45" t="s">
         <v>273</v>
-      </c>
-      <c r="O15" s="45" t="s">
-        <v>274</v>
       </c>
       <c r="P15" s="14"/>
       <c r="Q15" s="14"/>
@@ -11873,19 +11834,17 @@
     </row>
     <row r="16">
       <c r="A16" s="13" t="s">
+        <v>294</v>
+      </c>
+      <c r="B16" s="13" t="s">
         <v>295</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="C16" s="13" t="s">
         <v>296</v>
       </c>
-      <c r="C16" s="13" t="s">
-        <v>297</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>298</v>
-      </c>
-      <c r="E16" s="93" t="s">
-        <v>26</v>
+      <c r="D16" s="14"/>
+      <c r="E16" s="65" t="s">
+        <v>260</v>
       </c>
       <c r="F16" s="14"/>
       <c r="G16" s="14"/>
@@ -11900,10 +11859,10 @@
         <v>19</v>
       </c>
       <c r="N16" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="O16" s="45" t="s">
         <v>273</v>
-      </c>
-      <c r="O16" s="45" t="s">
-        <v>274</v>
       </c>
       <c r="P16" s="14"/>
       <c r="Q16" s="14"/>
@@ -11921,19 +11880,17 @@
     </row>
     <row r="17">
       <c r="A17" s="13" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>300</v>
-      </c>
-      <c r="D17" s="13" t="s">
+        <v>298</v>
+      </c>
+      <c r="D17" s="14"/>
+      <c r="E17" s="65" t="s">
         <v>260</v>
-      </c>
-      <c r="E17" s="93" t="s">
-        <v>26</v>
       </c>
       <c r="F17" s="14"/>
       <c r="G17" s="14"/>
@@ -11948,10 +11905,10 @@
         <v>19</v>
       </c>
       <c r="N17" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="O17" s="45" t="s">
         <v>273</v>
-      </c>
-      <c r="O17" s="45" t="s">
-        <v>274</v>
       </c>
       <c r="P17" s="14"/>
       <c r="Q17" s="14"/>
@@ -11969,19 +11926,17 @@
     </row>
     <row r="18">
       <c r="A18" s="13" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>302</v>
-      </c>
-      <c r="D18" s="13" t="s">
+        <v>300</v>
+      </c>
+      <c r="D18" s="14"/>
+      <c r="E18" s="65" t="s">
         <v>260</v>
-      </c>
-      <c r="E18" s="93" t="s">
-        <v>26</v>
       </c>
       <c r="F18" s="14"/>
       <c r="G18" s="14"/>
@@ -11996,10 +11951,10 @@
         <v>19</v>
       </c>
       <c r="N18" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="O18" s="45" t="s">
         <v>273</v>
-      </c>
-      <c r="O18" s="45" t="s">
-        <v>274</v>
       </c>
       <c r="P18" s="14"/>
       <c r="Q18" s="14"/>
@@ -12017,19 +11972,17 @@
     </row>
     <row r="19">
       <c r="A19" s="13" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>304</v>
-      </c>
-      <c r="D19" s="13" t="s">
+        <v>302</v>
+      </c>
+      <c r="D19" s="14"/>
+      <c r="E19" s="65" t="s">
         <v>260</v>
-      </c>
-      <c r="E19" s="93" t="s">
-        <v>26</v>
       </c>
       <c r="F19" s="14"/>
       <c r="G19" s="14"/>
@@ -12044,10 +11997,10 @@
         <v>19</v>
       </c>
       <c r="N19" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="O19" s="45" t="s">
         <v>273</v>
-      </c>
-      <c r="O19" s="45" t="s">
-        <v>274</v>
       </c>
       <c r="P19" s="14"/>
       <c r="Q19" s="14"/>
@@ -12065,25 +12018,23 @@
     </row>
     <row r="20">
       <c r="A20" s="13" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>306</v>
-      </c>
-      <c r="D20" s="13" t="s">
+        <v>304</v>
+      </c>
+      <c r="D20" s="14"/>
+      <c r="E20" s="65" t="s">
         <v>260</v>
-      </c>
-      <c r="E20" s="93" t="s">
-        <v>26</v>
       </c>
       <c r="F20" s="14"/>
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
       <c r="I20" s="13" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="J20" s="14"/>
       <c r="K20" s="15">
@@ -12094,10 +12045,10 @@
         <v>19</v>
       </c>
       <c r="N20" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="O20" s="45" t="s">
         <v>273</v>
-      </c>
-      <c r="O20" s="45" t="s">
-        <v>274</v>
       </c>
       <c r="P20" s="14"/>
       <c r="Q20" s="14"/>
@@ -12115,19 +12066,19 @@
     </row>
     <row r="21">
       <c r="A21" s="13" t="s">
+        <v>306</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>306</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>307</v>
+      </c>
+      <c r="D21" s="13" t="s">
         <v>308</v>
       </c>
-      <c r="B21" s="13" t="s">
-        <v>308</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>309</v>
-      </c>
-      <c r="D21" s="13" t="s">
-        <v>310</v>
-      </c>
-      <c r="E21" s="93" t="s">
-        <v>26</v>
+      <c r="E21" s="65" t="s">
+        <v>260</v>
       </c>
       <c r="F21" s="14"/>
       <c r="G21" s="14"/>
@@ -12142,10 +12093,10 @@
         <v>19</v>
       </c>
       <c r="N21" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="O21" s="45" t="s">
         <v>273</v>
-      </c>
-      <c r="O21" s="45" t="s">
-        <v>274</v>
       </c>
       <c r="P21" s="14"/>
       <c r="Q21" s="14"/>
@@ -12163,19 +12114,17 @@
     </row>
     <row r="22">
       <c r="A22" s="13" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>312</v>
-      </c>
-      <c r="D22" s="13" t="s">
+        <v>310</v>
+      </c>
+      <c r="D22" s="14"/>
+      <c r="E22" s="65" t="s">
         <v>260</v>
-      </c>
-      <c r="E22" s="93" t="s">
-        <v>26</v>
       </c>
       <c r="F22" s="14"/>
       <c r="G22" s="14"/>
@@ -12190,10 +12139,10 @@
         <v>19</v>
       </c>
       <c r="N22" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="O22" s="45" t="s">
         <v>273</v>
-      </c>
-      <c r="O22" s="45" t="s">
-        <v>274</v>
       </c>
       <c r="P22" s="14"/>
       <c r="Q22" s="14"/>
@@ -12211,19 +12160,19 @@
     </row>
     <row r="23">
       <c r="A23" s="13" t="s">
+        <v>311</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>312</v>
+      </c>
+      <c r="C23" s="13" t="s">
         <v>313</v>
       </c>
-      <c r="B23" s="13" t="s">
+      <c r="D23" s="13" t="s">
         <v>314</v>
       </c>
-      <c r="C23" s="13" t="s">
-        <v>315</v>
-      </c>
-      <c r="D23" s="13" t="s">
-        <v>316</v>
-      </c>
-      <c r="E23" s="93" t="s">
-        <v>26</v>
+      <c r="E23" s="65" t="s">
+        <v>260</v>
       </c>
       <c r="F23" s="14"/>
       <c r="G23" s="14"/>
@@ -12238,10 +12187,10 @@
         <v>19</v>
       </c>
       <c r="N23" s="13" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="O23" s="45" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="P23" s="14"/>
       <c r="Q23" s="14"/>
@@ -12259,19 +12208,19 @@
     </row>
     <row r="24">
       <c r="A24" s="13" t="s">
+        <v>317</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>318</v>
+      </c>
+      <c r="C24" s="13" t="s">
         <v>319</v>
       </c>
-      <c r="B24" s="13" t="s">
-        <v>320</v>
-      </c>
-      <c r="C24" s="13" t="s">
-        <v>321</v>
-      </c>
       <c r="D24" s="13" t="s">
-        <v>316</v>
-      </c>
-      <c r="E24" s="93" t="s">
-        <v>26</v>
+        <v>314</v>
+      </c>
+      <c r="E24" s="65" t="s">
+        <v>260</v>
       </c>
       <c r="F24" s="14"/>
       <c r="G24" s="14"/>
@@ -12286,10 +12235,10 @@
         <v>19</v>
       </c>
       <c r="N24" s="13" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="O24" s="45" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="P24" s="14"/>
       <c r="Q24" s="14"/>
@@ -12307,19 +12256,19 @@
     </row>
     <row r="25">
       <c r="A25" s="13" t="s">
+        <v>320</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>321</v>
+      </c>
+      <c r="C25" s="13" t="s">
         <v>322</v>
       </c>
-      <c r="B25" s="13" t="s">
-        <v>323</v>
-      </c>
-      <c r="C25" s="13" t="s">
-        <v>324</v>
-      </c>
       <c r="D25" s="13" t="s">
-        <v>316</v>
-      </c>
-      <c r="E25" s="93" t="s">
-        <v>26</v>
+        <v>314</v>
+      </c>
+      <c r="E25" s="65" t="s">
+        <v>260</v>
       </c>
       <c r="F25" s="14"/>
       <c r="G25" s="14"/>
@@ -12334,10 +12283,10 @@
         <v>19</v>
       </c>
       <c r="N25" s="13" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="O25" s="45" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="P25" s="14"/>
       <c r="Q25" s="14"/>
@@ -12355,19 +12304,17 @@
     </row>
     <row r="26">
       <c r="A26" s="13" t="s">
+        <v>323</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>324</v>
+      </c>
+      <c r="C26" s="13" t="s">
         <v>325</v>
       </c>
-      <c r="B26" s="13" t="s">
-        <v>326</v>
-      </c>
-      <c r="C26" s="13" t="s">
-        <v>327</v>
-      </c>
-      <c r="D26" s="13" t="s">
+      <c r="D26" s="14"/>
+      <c r="E26" s="65" t="s">
         <v>260</v>
-      </c>
-      <c r="E26" s="93" t="s">
-        <v>26</v>
       </c>
       <c r="F26" s="14"/>
       <c r="G26" s="14"/>
@@ -12382,10 +12329,10 @@
         <v>19</v>
       </c>
       <c r="N26" s="13" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="O26" s="45" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="P26" s="14"/>
       <c r="Q26" s="14"/>
@@ -12403,19 +12350,17 @@
     </row>
     <row r="27">
       <c r="A27" s="13" t="s">
+        <v>327</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>328</v>
+      </c>
+      <c r="C27" s="13" t="s">
         <v>329</v>
       </c>
-      <c r="B27" s="13" t="s">
-        <v>330</v>
-      </c>
-      <c r="C27" s="13" t="s">
-        <v>331</v>
-      </c>
-      <c r="D27" s="13" t="s">
+      <c r="D27" s="14"/>
+      <c r="E27" s="65" t="s">
         <v>260</v>
-      </c>
-      <c r="E27" s="93" t="s">
-        <v>26</v>
       </c>
       <c r="F27" s="14"/>
       <c r="G27" s="14"/>
@@ -12430,10 +12375,10 @@
         <v>19</v>
       </c>
       <c r="N27" s="13" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="O27" s="45" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="P27" s="14"/>
       <c r="Q27" s="14"/>

</xml_diff>

<commit_message>
WIP: fix parent relations, update RDF, HTML
</commit_message>
<xml_diff>
--- a/documentation-generator/vocab_csv/entities.xlsx
+++ b/documentation-generator/vocab_csv/entities.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="329">
   <si>
     <t>Term</t>
   </si>
@@ -144,6 +144,9 @@
     <t>A register containing information which is made publicly available</t>
   </si>
   <si>
+    <t>EDITORIAL: Registers can be for anything, e.g. data, so should be elsewhere?</t>
+  </si>
+  <si>
     <t>proposed</t>
   </si>
   <si>
@@ -255,7 +258,7 @@
     <t>An authority with the power to create or enforce laws, or determine their compliance.</t>
   </si>
   <si>
-    <t>dpv:LegalEntity,dpv:GovernmentalOrganisation</t>
+    <t>dpv:GovernmentalOrganisation</t>
   </si>
   <si>
     <t>Georg Krog, Paul Ryan, Harshvardhan Pandit</t>
@@ -399,7 +402,7 @@
     <t>Data Processor</t>
   </si>
   <si>
-    <t>A ‘processor’ means a natural or legal person, public authority, agency or other body which processes personal data on behalf of the controller.</t>
+    <t>A ‘processor’ means a natural or legal person, public authority, agency or other body which processes data on behalf of the controller.</t>
   </si>
   <si>
     <t>dpv:Recipient</t>
@@ -432,7 +435,7 @@
     <t>Recipient</t>
   </si>
   <si>
-    <t>Entities that receive personal data</t>
+    <t>Entities that receive data</t>
   </si>
   <si>
     <t>spl:AnyRecipient</t>
@@ -441,7 +444,7 @@
     <t>rdfs:seeAlso</t>
   </si>
   <si>
-    <t xml:space="preserve">A recipient of personal data can be used to indicate any entity that receives personal data. This can be a Third Party, Processor (GDPR), or even a Controller. </t>
+    <t xml:space="preserve">Recipients indicate entities that receives data, for example personal data recipients can be a Third Party, Data Controller, or Data Processor. </t>
   </si>
   <si>
     <r>
@@ -611,7 +614,7 @@
     <t>has recipient</t>
   </si>
   <si>
-    <t>Indicates Recipient of Personal Data</t>
+    <t>Indicates Recipient of Data</t>
   </si>
   <si>
     <t>(SPECIAL Project,https://specialprivacy.ercim.eu/)</t>
@@ -874,10 +877,7 @@
     <t>The individual (or category of individuals) whose personal data is being processed</t>
   </si>
   <si>
-    <t>dpv:LegalEntity,dpv:NaturalPerson</t>
-  </si>
-  <si>
-    <t>The term 'data subject' is specific to the GDPR, but is functionally equivalent to the term 'individual' and the ISO/IEC term 'PII Principle'.</t>
+    <t>The term 'data subject' is specific to the GDPR, but is functionally equivalent to the term 'individual associated with data' and the ISO/IEC term 'PII Principle'</t>
   </si>
   <si>
     <t>(GDPR Art.4-1g,https://eur-lex.europa.eu/eli/reg/2016/679/art_4/par_1/oj)</t>
@@ -1269,12 +1269,12 @@
     </font>
     <font>
       <u/>
-      <color rgb="FF000000"/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
-      <color rgb="FF000000"/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -1374,7 +1374,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="105">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1517,7 +1517,7 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="3" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="3" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
@@ -1553,7 +1553,7 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
@@ -1565,10 +1565,13 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="26" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
@@ -1627,11 +1630,17 @@
     <xf borderId="1" fillId="3" fontId="30" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="7" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="3" fontId="31" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
@@ -1642,23 +1651,29 @@
     <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
+    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="33" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf borderId="0" fillId="3" fontId="7" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="34" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf borderId="0" fillId="3" fontId="34" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
@@ -2291,12 +2306,14 @@
       <c r="F6" s="31"/>
       <c r="G6" s="29"/>
       <c r="H6" s="31"/>
-      <c r="I6" s="31"/>
+      <c r="I6" s="32" t="s">
+        <v>41</v>
+      </c>
       <c r="J6" s="29"/>
       <c r="K6" s="31"/>
       <c r="L6" s="31"/>
       <c r="M6" s="32" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="N6" s="31"/>
       <c r="O6" s="31"/>
@@ -2319,13 +2336,13 @@
     </row>
     <row r="7">
       <c r="A7" s="29" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B7" s="29" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D7" s="29" t="s">
         <v>38</v>
@@ -2339,7 +2356,7 @@
       <c r="K7" s="31"/>
       <c r="L7" s="31"/>
       <c r="M7" s="32" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="N7" s="31"/>
       <c r="O7" s="31"/>
@@ -5207,13 +5224,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
@@ -5228,7 +5245,7 @@
         <v>9</v>
       </c>
       <c r="K1" s="35" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="L1" s="6" t="s">
         <v>11</v>
@@ -5245,13 +5262,13 @@
     </row>
     <row r="2">
       <c r="A2" s="36" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B2" s="37" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C2" s="36" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D2" s="37" t="s">
         <v>25</v>
@@ -5260,7 +5277,7 @@
         <v>17</v>
       </c>
       <c r="F2" s="37" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G2" s="38"/>
       <c r="H2" s="39"/>
@@ -5274,7 +5291,7 @@
         <v>19</v>
       </c>
       <c r="N2" s="37" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="O2" s="42" t="s">
         <v>37</v>
@@ -5295,13 +5312,13 @@
     </row>
     <row r="3">
       <c r="A3" s="36" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B3" s="37" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C3" s="36" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D3" s="37" t="s">
         <v>25</v>
@@ -5310,7 +5327,7 @@
         <v>17</v>
       </c>
       <c r="F3" s="37" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G3" s="38"/>
       <c r="H3" s="39"/>
@@ -5324,7 +5341,7 @@
         <v>19</v>
       </c>
       <c r="N3" s="37" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="O3" s="42" t="s">
         <v>37</v>
@@ -5345,13 +5362,13 @@
     </row>
     <row r="4">
       <c r="A4" s="36" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B4" s="37" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C4" s="36" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D4" s="37" t="s">
         <v>25</v>
@@ -5360,7 +5377,7 @@
         <v>17</v>
       </c>
       <c r="F4" s="37" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G4" s="38"/>
       <c r="H4" s="39"/>
@@ -5374,7 +5391,7 @@
         <v>19</v>
       </c>
       <c r="N4" s="37" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="O4" s="42" t="s">
         <v>37</v>
@@ -5395,13 +5412,13 @@
     </row>
     <row r="5">
       <c r="A5" s="13" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>17</v>
@@ -5410,12 +5427,12 @@
         <v>25</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G5" s="14"/>
       <c r="H5" s="14"/>
       <c r="I5" s="13" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J5" s="14"/>
       <c r="K5" s="44">
@@ -5447,22 +5464,22 @@
     </row>
     <row r="6">
       <c r="A6" s="36" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B6" s="36" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C6" s="37" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D6" s="37" t="s">
         <v>25</v>
       </c>
       <c r="E6" s="37" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F6" s="37" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G6" s="37"/>
       <c r="H6" s="39"/>
@@ -5476,7 +5493,7 @@
         <v>19</v>
       </c>
       <c r="N6" s="37" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="O6" s="42" t="s">
         <v>37</v>
@@ -5497,13 +5514,13 @@
     </row>
     <row r="7">
       <c r="A7" s="13" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D7" s="13" t="s">
         <v>17</v>
@@ -5512,7 +5529,7 @@
         <v>25</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
@@ -5529,7 +5546,7 @@
         <v>20</v>
       </c>
       <c r="O7" s="46" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="P7" s="14"/>
       <c r="Q7" s="14"/>
@@ -5547,22 +5564,22 @@
     </row>
     <row r="8">
       <c r="A8" s="13" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E8" s="13" t="s">
         <v>25</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G8" s="14"/>
       <c r="H8" s="14"/>
@@ -5704,16 +5721,16 @@
     </row>
     <row r="2">
       <c r="A2" s="47" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B2" s="48" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C2" s="48" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D2" s="49" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E2" s="50" t="s">
         <v>26</v>
@@ -5731,7 +5748,7 @@
         <v>19</v>
       </c>
       <c r="N2" s="48" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="O2" s="53" t="s">
         <v>37</v>
@@ -5752,16 +5769,16 @@
     </row>
     <row r="3">
       <c r="A3" s="47" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B3" s="54" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C3" s="48" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D3" s="48" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E3" s="55" t="s">
         <v>26</v>
@@ -5779,7 +5796,7 @@
         <v>19</v>
       </c>
       <c r="N3" s="48" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="O3" s="53" t="s">
         <v>37</v>
@@ -5800,16 +5817,16 @@
     </row>
     <row r="4">
       <c r="A4" s="48" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4" s="55" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" s="55" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" s="48" t="s">
         <v>84</v>
-      </c>
-      <c r="B4" s="55" t="s">
-        <v>85</v>
-      </c>
-      <c r="C4" s="55" t="s">
-        <v>86</v>
-      </c>
-      <c r="D4" s="48" t="s">
-        <v>83</v>
       </c>
       <c r="E4" s="22" t="s">
         <v>26</v>
@@ -5819,7 +5836,7 @@
       <c r="H4" s="23"/>
       <c r="I4" s="56"/>
       <c r="J4" s="57" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="K4" s="52">
         <v>44594.0</v>
@@ -5850,16 +5867,16 @@
     </row>
     <row r="5">
       <c r="A5" s="54" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B5" s="55" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C5" s="55" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D5" s="54" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E5" s="22" t="s">
         <v>26</v>
@@ -5869,7 +5886,7 @@
       <c r="H5" s="23"/>
       <c r="I5" s="23"/>
       <c r="J5" s="57" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="K5" s="52">
         <v>44594.0</v>
@@ -5900,16 +5917,16 @@
     </row>
     <row r="6">
       <c r="A6" s="48" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B6" s="55" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C6" s="55" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D6" s="48" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E6" s="22" t="s">
         <v>26</v>
@@ -5919,7 +5936,7 @@
       <c r="H6" s="23"/>
       <c r="I6" s="23"/>
       <c r="J6" s="58" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="K6" s="52">
         <v>44594.0</v>
@@ -8795,13 +8812,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
@@ -8816,7 +8833,7 @@
         <v>9</v>
       </c>
       <c r="K1" s="35" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="L1" s="6" t="s">
         <v>11</v>
@@ -8833,19 +8850,19 @@
     </row>
     <row r="2">
       <c r="A2" s="36" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B2" s="37" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C2" s="36" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D2" s="37" t="s">
         <v>17</v>
       </c>
       <c r="E2" s="37" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F2" s="43"/>
       <c r="G2" s="38"/>
@@ -8860,10 +8877,10 @@
         <v>19</v>
       </c>
       <c r="N2" s="37" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="O2" s="42" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="P2" s="43"/>
       <c r="Q2" s="43"/>
@@ -8881,16 +8898,16 @@
     </row>
     <row r="3">
       <c r="A3" s="13" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E3" s="13" t="s">
         <v>17</v>
@@ -8908,10 +8925,10 @@
         <v>19</v>
       </c>
       <c r="N3" s="13" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="O3" s="42" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="P3" s="14"/>
       <c r="Q3" s="14"/>
@@ -9035,13 +9052,13 @@
     </row>
     <row r="2">
       <c r="A2" s="59" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B2" s="60" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C2" s="61" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D2" s="59" t="s">
         <v>34</v>
@@ -9053,10 +9070,10 @@
       <c r="G2" s="23"/>
       <c r="H2" s="23"/>
       <c r="I2" s="62" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="J2" s="63" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="K2" s="25">
         <v>43560.0</v>
@@ -9068,7 +9085,7 @@
         <v>19</v>
       </c>
       <c r="N2" s="59" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="O2" s="27" t="s">
         <v>27</v>
@@ -9089,16 +9106,16 @@
     </row>
     <row r="3">
       <c r="A3" s="13" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E3" s="13" t="s">
         <v>26</v>
@@ -9108,7 +9125,7 @@
       <c r="H3" s="14"/>
       <c r="I3" s="14"/>
       <c r="J3" s="64" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="K3" s="15">
         <v>43620.0</v>
@@ -9121,7 +9138,7 @@
         <v>20</v>
       </c>
       <c r="O3" s="45" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="P3" s="14"/>
       <c r="Q3" s="14"/>
@@ -9139,16 +9156,16 @@
     </row>
     <row r="4">
       <c r="A4" s="13" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E4" s="13" t="s">
         <v>26</v>
@@ -9157,7 +9174,7 @@
       <c r="G4" s="14"/>
       <c r="H4" s="14"/>
       <c r="I4" s="13" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="J4" s="14"/>
       <c r="K4" s="15">
@@ -9171,7 +9188,7 @@
         <v>20</v>
       </c>
       <c r="O4" s="45" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="P4" s="14"/>
       <c r="Q4" s="14"/>
@@ -9189,13 +9206,13 @@
     </row>
     <row r="5">
       <c r="A5" s="59" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B5" s="60" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C5" s="61" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D5" s="59" t="s">
         <v>34</v>
@@ -9205,28 +9222,28 @@
       </c>
       <c r="F5" s="21"/>
       <c r="G5" s="21" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H5" s="21" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="I5" s="65" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="J5" s="66" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="K5" s="25">
         <v>43560.0</v>
       </c>
-      <c r="L5" s="25">
-        <v>44139.0</v>
+      <c r="L5" s="67">
+        <v>45270.0</v>
       </c>
       <c r="M5" s="59" t="s">
         <v>19</v>
       </c>
       <c r="N5" s="59" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="O5" s="27" t="s">
         <v>27</v>
@@ -9247,16 +9264,16 @@
     </row>
     <row r="6">
       <c r="A6" s="13" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E6" s="13" t="s">
         <v>26</v>
@@ -9266,7 +9283,7 @@
       <c r="H6" s="14"/>
       <c r="I6" s="14"/>
       <c r="J6" s="64" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="K6" s="15">
         <v>43620.0</v>
@@ -9279,7 +9296,7 @@
         <v>20</v>
       </c>
       <c r="O6" s="45" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="P6" s="14"/>
       <c r="Q6" s="14"/>
@@ -9297,13 +9314,13 @@
     </row>
     <row r="7">
       <c r="A7" s="13" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D7" s="13" t="s">
         <v>34</v>
@@ -9315,10 +9332,10 @@
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
       <c r="I7" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="J7" s="67" t="s">
         <v>136</v>
+      </c>
+      <c r="J7" s="68" t="s">
+        <v>137</v>
       </c>
       <c r="K7" s="15">
         <v>44447.0</v>
@@ -9328,10 +9345,10 @@
         <v>19</v>
       </c>
       <c r="N7" s="37" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="O7" s="45" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="P7" s="14"/>
       <c r="Q7" s="14"/>
@@ -9349,16 +9366,16 @@
     </row>
     <row r="8">
       <c r="A8" s="13" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E8" s="13" t="s">
         <v>26</v>
@@ -9366,11 +9383,11 @@
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
       <c r="H8" s="14"/>
-      <c r="I8" s="68" t="s">
-        <v>142</v>
-      </c>
-      <c r="J8" s="67" t="s">
+      <c r="I8" s="69" t="s">
         <v>143</v>
+      </c>
+      <c r="J8" s="68" t="s">
+        <v>144</v>
       </c>
       <c r="K8" s="15">
         <v>44447.0</v>
@@ -9380,10 +9397,10 @@
         <v>19</v>
       </c>
       <c r="N8" s="37" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="O8" s="45" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="P8" s="14"/>
       <c r="Q8" s="14"/>
@@ -9401,16 +9418,16 @@
     </row>
     <row r="9">
       <c r="A9" s="13" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E9" s="13" t="s">
         <v>26</v>
@@ -9419,7 +9436,7 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
       <c r="I9" s="13" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="J9" s="14"/>
       <c r="K9" s="15">
@@ -9430,7 +9447,7 @@
         <v>19</v>
       </c>
       <c r="N9" s="37" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="O9" s="45" t="s">
         <v>21</v>
@@ -9450,56 +9467,56 @@
       <c r="AB9" s="14"/>
     </row>
     <row r="10">
-      <c r="A10" s="69" t="s">
-        <v>150</v>
-      </c>
-      <c r="B10" s="69" t="s">
+      <c r="A10" s="70" t="s">
         <v>151</v>
       </c>
-      <c r="C10" s="70" t="s">
+      <c r="B10" s="70" t="s">
         <v>152</v>
       </c>
-      <c r="D10" s="71" t="s">
-        <v>67</v>
-      </c>
-      <c r="E10" s="72" t="s">
+      <c r="C10" s="71" t="s">
+        <v>153</v>
+      </c>
+      <c r="D10" s="72" t="s">
+        <v>68</v>
+      </c>
+      <c r="E10" s="73" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="73"/>
-      <c r="G10" s="73"/>
-      <c r="H10" s="73"/>
-      <c r="I10" s="73"/>
-      <c r="J10" s="74" t="s">
-        <v>153</v>
-      </c>
-      <c r="K10" s="75">
+      <c r="F10" s="74"/>
+      <c r="G10" s="74"/>
+      <c r="H10" s="74"/>
+      <c r="I10" s="74"/>
+      <c r="J10" s="75" t="s">
+        <v>154</v>
+      </c>
+      <c r="K10" s="76">
         <v>44139.0</v>
       </c>
-      <c r="L10" s="75">
+      <c r="L10" s="76">
         <v>44538.0</v>
       </c>
-      <c r="M10" s="76" t="s">
+      <c r="M10" s="77" t="s">
         <v>19</v>
       </c>
-      <c r="N10" s="70" t="s">
-        <v>154</v>
-      </c>
-      <c r="O10" s="77" t="s">
+      <c r="N10" s="71" t="s">
+        <v>155</v>
+      </c>
+      <c r="O10" s="78" t="s">
         <v>37</v>
       </c>
-      <c r="P10" s="78"/>
-      <c r="Q10" s="78"/>
-      <c r="R10" s="73"/>
-      <c r="S10" s="73"/>
-      <c r="T10" s="73"/>
-      <c r="U10" s="73"/>
-      <c r="V10" s="73"/>
-      <c r="W10" s="73"/>
-      <c r="X10" s="73"/>
-      <c r="Y10" s="73"/>
-      <c r="Z10" s="73"/>
-      <c r="AA10" s="73"/>
-      <c r="AB10" s="73"/>
+      <c r="P10" s="79"/>
+      <c r="Q10" s="79"/>
+      <c r="R10" s="74"/>
+      <c r="S10" s="74"/>
+      <c r="T10" s="74"/>
+      <c r="U10" s="74"/>
+      <c r="V10" s="74"/>
+      <c r="W10" s="74"/>
+      <c r="X10" s="74"/>
+      <c r="Y10" s="74"/>
+      <c r="Z10" s="74"/>
+      <c r="AA10" s="74"/>
+      <c r="AB10" s="74"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:AB10">
@@ -9566,13 +9583,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
@@ -9587,7 +9604,7 @@
         <v>9</v>
       </c>
       <c r="K1" s="35" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="L1" s="6" t="s">
         <v>11</v>
@@ -9603,42 +9620,42 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="79" t="s">
-        <v>155</v>
-      </c>
-      <c r="B2" s="79" t="s">
+      <c r="A2" s="80" t="s">
         <v>156</v>
       </c>
-      <c r="C2" s="80" t="s">
+      <c r="B2" s="80" t="s">
         <v>157</v>
       </c>
-      <c r="D2" s="79" t="s">
+      <c r="C2" s="81" t="s">
+        <v>158</v>
+      </c>
+      <c r="D2" s="80" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="79" t="str">
+      <c r="E2" s="80" t="str">
         <f>CONCATENATE("dpv:",RIGHT(A2,LEN(A2) - 3))</f>
         <v>dpv:DataController</v>
       </c>
       <c r="F2" s="21" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G2" s="23"/>
       <c r="H2" s="23"/>
       <c r="I2" s="23"/>
-      <c r="J2" s="79"/>
-      <c r="K2" s="81">
+      <c r="J2" s="80"/>
+      <c r="K2" s="82">
         <v>43559.0</v>
       </c>
-      <c r="L2" s="81">
+      <c r="L2" s="82">
         <v>44139.0</v>
       </c>
-      <c r="M2" s="79" t="s">
+      <c r="M2" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="N2" s="79" t="s">
-        <v>158</v>
-      </c>
-      <c r="O2" s="82" t="s">
+      <c r="N2" s="80" t="s">
+        <v>159</v>
+      </c>
+      <c r="O2" s="83" t="s">
         <v>27</v>
       </c>
       <c r="P2" s="28"/>
@@ -9657,28 +9674,28 @@
     </row>
     <row r="3">
       <c r="A3" s="21" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D3" s="21" t="s">
         <v>17</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>162</v>
-      </c>
-      <c r="F3" s="83" t="s">
         <v>163</v>
+      </c>
+      <c r="F3" s="84" t="s">
+        <v>164</v>
       </c>
       <c r="G3" s="23"/>
       <c r="H3" s="23"/>
       <c r="I3" s="23"/>
       <c r="J3" s="23"/>
-      <c r="K3" s="84">
+      <c r="K3" s="85">
         <v>44601.0</v>
       </c>
       <c r="L3" s="23"/>
@@ -9686,9 +9703,9 @@
         <v>19</v>
       </c>
       <c r="N3" s="21" t="s">
-        <v>164</v>
-      </c>
-      <c r="O3" s="85" t="s">
+        <v>165</v>
+      </c>
+      <c r="O3" s="86" t="s">
         <v>31</v>
       </c>
       <c r="P3" s="28"/>
@@ -9707,28 +9724,28 @@
     </row>
     <row r="4">
       <c r="A4" s="21" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D4" s="21" t="s">
         <v>17</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>119</v>
-      </c>
-      <c r="F4" s="83" t="s">
-        <v>168</v>
+        <v>120</v>
+      </c>
+      <c r="F4" s="84" t="s">
+        <v>169</v>
       </c>
       <c r="G4" s="23"/>
       <c r="H4" s="23"/>
       <c r="I4" s="23"/>
       <c r="J4" s="23"/>
-      <c r="K4" s="84">
+      <c r="K4" s="85">
         <v>44601.0</v>
       </c>
       <c r="L4" s="23"/>
@@ -9736,9 +9753,9 @@
         <v>19</v>
       </c>
       <c r="N4" s="21" t="s">
-        <v>164</v>
-      </c>
-      <c r="O4" s="85" t="s">
+        <v>165</v>
+      </c>
+      <c r="O4" s="86" t="s">
         <v>31</v>
       </c>
       <c r="P4" s="28"/>
@@ -9757,28 +9774,28 @@
     </row>
     <row r="5">
       <c r="A5" s="13" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>170</v>
-      </c>
-      <c r="C5" s="13" t="s">
         <v>171</v>
+      </c>
+      <c r="C5" s="87" t="s">
+        <v>172</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>17</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G5" s="14"/>
       <c r="H5" s="14"/>
       <c r="I5" s="14"/>
       <c r="J5" s="13" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="K5" s="15">
         <v>43559.0</v>
@@ -9790,7 +9807,7 @@
         <v>19</v>
       </c>
       <c r="N5" s="13" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="O5" s="45" t="s">
         <v>27</v>
@@ -9811,28 +9828,28 @@
     </row>
     <row r="6">
       <c r="A6" s="21" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D6" s="21" t="s">
         <v>17</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>147</v>
-      </c>
-      <c r="F6" s="83" t="s">
-        <v>168</v>
+        <v>148</v>
+      </c>
+      <c r="F6" s="84" t="s">
+        <v>169</v>
       </c>
       <c r="G6" s="23"/>
       <c r="H6" s="23"/>
       <c r="I6" s="23"/>
       <c r="J6" s="23"/>
-      <c r="K6" s="84">
+      <c r="K6" s="85">
         <v>44601.0</v>
       </c>
       <c r="L6" s="23"/>
@@ -9840,9 +9857,9 @@
         <v>19</v>
       </c>
       <c r="N6" s="21" t="s">
-        <v>164</v>
-      </c>
-      <c r="O6" s="85" t="s">
+        <v>165</v>
+      </c>
+      <c r="O6" s="86" t="s">
         <v>31</v>
       </c>
       <c r="P6" s="28"/>
@@ -9861,28 +9878,28 @@
     </row>
     <row r="7">
       <c r="A7" s="21" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D7" s="21" t="s">
         <v>17</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>180</v>
-      </c>
-      <c r="F7" s="83" t="s">
-        <v>168</v>
+        <v>181</v>
+      </c>
+      <c r="F7" s="84" t="s">
+        <v>169</v>
       </c>
       <c r="G7" s="23"/>
       <c r="H7" s="23"/>
       <c r="I7" s="23"/>
       <c r="J7" s="23"/>
-      <c r="K7" s="84">
+      <c r="K7" s="85">
         <v>44601.0</v>
       </c>
       <c r="L7" s="23"/>
@@ -9890,9 +9907,9 @@
         <v>19</v>
       </c>
       <c r="N7" s="21" t="s">
-        <v>164</v>
-      </c>
-      <c r="O7" s="85" t="s">
+        <v>165</v>
+      </c>
+      <c r="O7" s="86" t="s">
         <v>31</v>
       </c>
       <c r="P7" s="28"/>
@@ -9911,28 +9928,28 @@
     </row>
     <row r="8">
       <c r="A8" s="21" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D8" s="21" t="s">
         <v>17</v>
       </c>
       <c r="E8" s="21" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="F8" s="21" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G8" s="23"/>
       <c r="H8" s="23"/>
       <c r="I8" s="23"/>
       <c r="J8" s="23"/>
-      <c r="K8" s="84">
+      <c r="K8" s="85">
         <v>44601.0</v>
       </c>
       <c r="L8" s="23"/>
@@ -9940,9 +9957,9 @@
         <v>19</v>
       </c>
       <c r="N8" s="21" t="s">
-        <v>164</v>
-      </c>
-      <c r="O8" s="85" t="s">
+        <v>165</v>
+      </c>
+      <c r="O8" s="86" t="s">
         <v>31</v>
       </c>
       <c r="P8" s="28"/>
@@ -9961,28 +9978,28 @@
     </row>
     <row r="9">
       <c r="A9" s="21" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D9" s="21" t="s">
         <v>17</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>188</v>
-      </c>
-      <c r="F9" s="83" t="s">
-        <v>168</v>
+        <v>189</v>
+      </c>
+      <c r="F9" s="84" t="s">
+        <v>169</v>
       </c>
       <c r="G9" s="23"/>
       <c r="H9" s="23"/>
       <c r="I9" s="23"/>
       <c r="J9" s="23"/>
-      <c r="K9" s="84">
+      <c r="K9" s="85">
         <v>44601.0</v>
       </c>
       <c r="L9" s="23"/>
@@ -9990,9 +10007,9 @@
         <v>19</v>
       </c>
       <c r="N9" s="21" t="s">
-        <v>164</v>
-      </c>
-      <c r="O9" s="85" t="s">
+        <v>165</v>
+      </c>
+      <c r="O9" s="86" t="s">
         <v>31</v>
       </c>
       <c r="P9" s="28"/>
@@ -10011,22 +10028,22 @@
     </row>
     <row r="10">
       <c r="A10" s="21" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D10" s="21" t="s">
         <v>17</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>192</v>
-      </c>
-      <c r="F10" s="83" t="s">
         <v>193</v>
+      </c>
+      <c r="F10" s="84" t="s">
+        <v>194</v>
       </c>
       <c r="G10" s="23"/>
       <c r="H10" s="23"/>
@@ -10040,10 +10057,10 @@
         <v>19</v>
       </c>
       <c r="N10" s="21" t="s">
-        <v>194</v>
-      </c>
-      <c r="O10" s="85" t="s">
-        <v>72</v>
+        <v>195</v>
+      </c>
+      <c r="O10" s="86" t="s">
+        <v>73</v>
       </c>
       <c r="P10" s="28"/>
       <c r="Q10" s="28"/>
@@ -10154,13 +10171,13 @@
     </row>
     <row r="2">
       <c r="A2" s="21" t="s">
-        <v>195</v>
-      </c>
-      <c r="B2" s="79" t="s">
-        <v>195</v>
+        <v>196</v>
+      </c>
+      <c r="B2" s="80" t="s">
+        <v>196</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D2" s="21" t="s">
         <v>34</v>
@@ -10183,7 +10200,7 @@
       <c r="N2" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="O2" s="83" t="s">
+      <c r="O2" s="84" t="s">
         <v>21</v>
       </c>
       <c r="P2" s="28"/>
@@ -10202,16 +10219,16 @@
     </row>
     <row r="3">
       <c r="A3" s="21" t="s">
-        <v>197</v>
-      </c>
-      <c r="B3" s="86" t="s">
         <v>198</v>
       </c>
+      <c r="B3" s="88" t="s">
+        <v>199</v>
+      </c>
       <c r="C3" s="21" t="s">
-        <v>199</v>
-      </c>
-      <c r="D3" s="83" t="s">
         <v>200</v>
+      </c>
+      <c r="D3" s="84" t="s">
+        <v>201</v>
       </c>
       <c r="E3" s="22" t="s">
         <v>26</v>
@@ -10221,12 +10238,12 @@
       <c r="H3" s="23"/>
       <c r="I3" s="23"/>
       <c r="J3" s="21" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="K3" s="25">
         <v>44594.0</v>
       </c>
-      <c r="L3" s="87">
+      <c r="L3" s="89">
         <v>44109.0</v>
       </c>
       <c r="M3" s="21" t="s">
@@ -10235,7 +10252,7 @@
       <c r="N3" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="O3" s="83" t="s">
+      <c r="O3" s="84" t="s">
         <v>21</v>
       </c>
       <c r="P3" s="28"/>
@@ -10254,16 +10271,16 @@
     </row>
     <row r="4">
       <c r="A4" s="21" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B4" s="62" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>204</v>
-      </c>
-      <c r="D4" s="83" t="s">
-        <v>200</v>
+        <v>205</v>
+      </c>
+      <c r="D4" s="84" t="s">
+        <v>201</v>
       </c>
       <c r="E4" s="22" t="s">
         <v>26</v>
@@ -10276,7 +10293,7 @@
       <c r="K4" s="25">
         <v>44594.0</v>
       </c>
-      <c r="L4" s="87">
+      <c r="L4" s="89">
         <v>44109.0</v>
       </c>
       <c r="M4" s="21" t="s">
@@ -10285,7 +10302,7 @@
       <c r="N4" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="O4" s="83" t="s">
+      <c r="O4" s="84" t="s">
         <v>21</v>
       </c>
       <c r="P4" s="28"/>
@@ -10304,16 +10321,16 @@
     </row>
     <row r="5">
       <c r="A5" s="21" t="s">
-        <v>205</v>
-      </c>
-      <c r="B5" s="86" t="s">
         <v>206</v>
       </c>
+      <c r="B5" s="88" t="s">
+        <v>207</v>
+      </c>
       <c r="C5" s="21" t="s">
-        <v>207</v>
-      </c>
-      <c r="D5" s="83" t="s">
-        <v>200</v>
+        <v>208</v>
+      </c>
+      <c r="D5" s="84" t="s">
+        <v>201</v>
       </c>
       <c r="E5" s="22" t="s">
         <v>26</v>
@@ -10323,12 +10340,12 @@
       <c r="H5" s="23"/>
       <c r="I5" s="23"/>
       <c r="J5" s="21" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="K5" s="25">
         <v>44594.0</v>
       </c>
-      <c r="L5" s="87">
+      <c r="L5" s="89">
         <v>44109.0</v>
       </c>
       <c r="M5" s="21" t="s">
@@ -10337,7 +10354,7 @@
       <c r="N5" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="O5" s="83" t="s">
+      <c r="O5" s="84" t="s">
         <v>21</v>
       </c>
       <c r="P5" s="28"/>
@@ -10356,16 +10373,16 @@
     </row>
     <row r="6">
       <c r="A6" s="21" t="s">
-        <v>208</v>
-      </c>
-      <c r="B6" s="86" t="s">
         <v>209</v>
       </c>
+      <c r="B6" s="88" t="s">
+        <v>210</v>
+      </c>
       <c r="C6" s="21" t="s">
-        <v>210</v>
-      </c>
-      <c r="D6" s="83" t="s">
-        <v>200</v>
+        <v>211</v>
+      </c>
+      <c r="D6" s="84" t="s">
+        <v>201</v>
       </c>
       <c r="E6" s="22" t="s">
         <v>26</v>
@@ -10378,7 +10395,7 @@
       <c r="K6" s="25">
         <v>44594.0</v>
       </c>
-      <c r="L6" s="87">
+      <c r="L6" s="89">
         <v>44109.0</v>
       </c>
       <c r="M6" s="21" t="s">
@@ -10387,7 +10404,7 @@
       <c r="N6" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="O6" s="83" t="s">
+      <c r="O6" s="84" t="s">
         <v>21</v>
       </c>
       <c r="P6" s="28"/>
@@ -10406,16 +10423,16 @@
     </row>
     <row r="7">
       <c r="A7" s="21" t="s">
-        <v>211</v>
-      </c>
-      <c r="B7" s="86" t="s">
         <v>212</v>
       </c>
+      <c r="B7" s="88" t="s">
+        <v>213</v>
+      </c>
       <c r="C7" s="21" t="s">
-        <v>213</v>
-      </c>
-      <c r="D7" s="83" t="s">
-        <v>200</v>
+        <v>214</v>
+      </c>
+      <c r="D7" s="84" t="s">
+        <v>201</v>
       </c>
       <c r="E7" s="22" t="s">
         <v>26</v>
@@ -10425,12 +10442,12 @@
       <c r="H7" s="23"/>
       <c r="I7" s="23"/>
       <c r="J7" s="21" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="K7" s="25">
         <v>44594.0</v>
       </c>
-      <c r="L7" s="87">
+      <c r="L7" s="89">
         <v>44109.0</v>
       </c>
       <c r="M7" s="21" t="s">
@@ -10439,7 +10456,7 @@
       <c r="N7" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="O7" s="83" t="s">
+      <c r="O7" s="84" t="s">
         <v>21</v>
       </c>
       <c r="P7" s="28"/>
@@ -10458,16 +10475,16 @@
     </row>
     <row r="8">
       <c r="A8" s="21" t="s">
-        <v>214</v>
-      </c>
-      <c r="B8" s="86" t="s">
         <v>215</v>
       </c>
+      <c r="B8" s="88" t="s">
+        <v>216</v>
+      </c>
       <c r="C8" s="21" t="s">
-        <v>216</v>
-      </c>
-      <c r="D8" s="83" t="s">
-        <v>200</v>
+        <v>217</v>
+      </c>
+      <c r="D8" s="84" t="s">
+        <v>201</v>
       </c>
       <c r="E8" s="22" t="s">
         <v>26</v>
@@ -10477,12 +10494,12 @@
       <c r="H8" s="23"/>
       <c r="I8" s="23"/>
       <c r="J8" s="21" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="K8" s="25">
         <v>44594.0</v>
       </c>
-      <c r="L8" s="87">
+      <c r="L8" s="89">
         <v>44109.0</v>
       </c>
       <c r="M8" s="21" t="s">
@@ -10491,7 +10508,7 @@
       <c r="N8" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="O8" s="83" t="s">
+      <c r="O8" s="84" t="s">
         <v>21</v>
       </c>
       <c r="P8" s="28"/>
@@ -10510,16 +10527,16 @@
     </row>
     <row r="9">
       <c r="A9" s="48" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B9" s="48" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C9" s="48" t="s">
-        <v>219</v>
-      </c>
-      <c r="D9" s="49" t="s">
-        <v>200</v>
+        <v>220</v>
+      </c>
+      <c r="D9" s="90" t="s">
+        <v>201</v>
       </c>
       <c r="E9" s="22" t="s">
         <v>26</v>
@@ -10529,22 +10546,22 @@
       <c r="H9" s="23"/>
       <c r="I9" s="23"/>
       <c r="J9" s="57" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="K9" s="52">
         <v>44643.0</v>
       </c>
-      <c r="L9" s="87">
+      <c r="L9" s="89">
         <v>44109.0</v>
       </c>
       <c r="M9" s="21" t="s">
         <v>19</v>
       </c>
       <c r="N9" s="48" t="s">
-        <v>221</v>
-      </c>
-      <c r="O9" s="88" t="s">
         <v>222</v>
+      </c>
+      <c r="O9" s="91" t="s">
+        <v>223</v>
       </c>
       <c r="P9" s="28"/>
       <c r="Q9" s="28"/>
@@ -10562,13 +10579,13 @@
     </row>
     <row r="10">
       <c r="A10" s="48" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B10" s="48" t="s">
-        <v>224</v>
-      </c>
-      <c r="C10" s="49" t="s">
         <v>225</v>
+      </c>
+      <c r="C10" s="90" t="s">
+        <v>226</v>
       </c>
       <c r="D10" s="22" t="s">
         <v>25</v>
@@ -10589,10 +10606,10 @@
         <v>19</v>
       </c>
       <c r="N10" s="48" t="s">
-        <v>226</v>
-      </c>
-      <c r="O10" s="88" t="s">
-        <v>222</v>
+        <v>227</v>
+      </c>
+      <c r="O10" s="91" t="s">
+        <v>223</v>
       </c>
       <c r="P10" s="28"/>
       <c r="Q10" s="28"/>
@@ -10609,11 +10626,11 @@
       <c r="AB10" s="23"/>
     </row>
     <row r="11">
-      <c r="A11" s="89" t="s">
-        <v>227</v>
-      </c>
-      <c r="B11" s="89" t="s">
+      <c r="A11" s="92" t="s">
         <v>228</v>
+      </c>
+      <c r="B11" s="92" t="s">
+        <v>229</v>
       </c>
       <c r="C11" s="14"/>
       <c r="D11" s="13" t="s">
@@ -10630,7 +10647,7 @@
       <c r="K11" s="14"/>
       <c r="L11" s="14"/>
       <c r="M11" s="13" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="N11" s="14"/>
       <c r="O11" s="14"/>
@@ -10649,11 +10666,11 @@
       <c r="AB11" s="14"/>
     </row>
     <row r="12">
-      <c r="A12" s="89" t="s">
-        <v>229</v>
-      </c>
-      <c r="B12" s="89" t="s">
+      <c r="A12" s="92" t="s">
         <v>230</v>
+      </c>
+      <c r="B12" s="92" t="s">
+        <v>231</v>
       </c>
       <c r="C12" s="14"/>
       <c r="D12" s="13" t="s">
@@ -10670,7 +10687,7 @@
       <c r="K12" s="14"/>
       <c r="L12" s="14"/>
       <c r="M12" s="13" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="N12" s="14"/>
       <c r="O12" s="14"/>
@@ -10689,11 +10706,11 @@
       <c r="AB12" s="14"/>
     </row>
     <row r="13">
-      <c r="A13" s="89" t="s">
-        <v>231</v>
-      </c>
-      <c r="B13" s="89" t="s">
+      <c r="A13" s="92" t="s">
         <v>232</v>
+      </c>
+      <c r="B13" s="92" t="s">
+        <v>233</v>
       </c>
       <c r="C13" s="14"/>
       <c r="D13" s="13" t="s">
@@ -10710,7 +10727,7 @@
       <c r="K13" s="14"/>
       <c r="L13" s="14"/>
       <c r="M13" s="13" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="N13" s="14"/>
       <c r="O13" s="14"/>
@@ -10729,11 +10746,11 @@
       <c r="AB13" s="14"/>
     </row>
     <row r="14">
-      <c r="A14" s="89" t="s">
-        <v>233</v>
-      </c>
-      <c r="B14" s="89" t="s">
+      <c r="A14" s="92" t="s">
         <v>234</v>
+      </c>
+      <c r="B14" s="92" t="s">
+        <v>235</v>
       </c>
       <c r="C14" s="14"/>
       <c r="D14" s="13" t="s">
@@ -10750,7 +10767,7 @@
       <c r="K14" s="14"/>
       <c r="L14" s="14"/>
       <c r="M14" s="13" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="N14" s="14"/>
       <c r="O14" s="14"/>
@@ -10769,11 +10786,11 @@
       <c r="AB14" s="14"/>
     </row>
     <row r="15">
-      <c r="A15" s="89" t="s">
-        <v>235</v>
-      </c>
-      <c r="B15" s="89" t="s">
+      <c r="A15" s="92" t="s">
         <v>236</v>
+      </c>
+      <c r="B15" s="92" t="s">
+        <v>237</v>
       </c>
       <c r="C15" s="14"/>
       <c r="D15" s="13" t="s">
@@ -10790,7 +10807,7 @@
       <c r="K15" s="14"/>
       <c r="L15" s="14"/>
       <c r="M15" s="13" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="N15" s="14"/>
       <c r="O15" s="14"/>
@@ -10810,16 +10827,16 @@
     </row>
     <row r="16">
       <c r="A16" s="36" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B16" s="37" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D16" s="37" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="E16" s="37" t="s">
         <v>26</v>
@@ -10832,7 +10849,7 @@
       <c r="K16" s="40"/>
       <c r="L16" s="40"/>
       <c r="M16" s="37" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="N16" s="37"/>
       <c r="O16" s="37"/>
@@ -10898,17 +10915,17 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="90" t="s">
+      <c r="C1" s="93" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
@@ -10923,7 +10940,7 @@
         <v>9</v>
       </c>
       <c r="K1" s="35" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="L1" s="6" t="s">
         <v>11</v>
@@ -10939,42 +10956,42 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="79" t="s">
-        <v>240</v>
-      </c>
-      <c r="B2" s="79" t="s">
+      <c r="A2" s="80" t="s">
         <v>241</v>
       </c>
-      <c r="C2" s="79" t="s">
+      <c r="B2" s="80" t="s">
         <v>242</v>
       </c>
-      <c r="D2" s="79" t="s">
+      <c r="C2" s="80" t="s">
+        <v>243</v>
+      </c>
+      <c r="D2" s="80" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="79" t="str">
+      <c r="E2" s="80" t="str">
         <f>CONCATENATE("dpv:",RIGHT(A2,LEN(A2) - 3))</f>
         <v>dpv:DataSubject</v>
       </c>
       <c r="F2" s="59" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G2" s="23"/>
       <c r="H2" s="23"/>
       <c r="I2" s="23"/>
-      <c r="J2" s="79"/>
-      <c r="K2" s="81">
+      <c r="J2" s="80"/>
+      <c r="K2" s="82">
         <v>43559.0</v>
       </c>
-      <c r="L2" s="81">
+      <c r="L2" s="82">
         <v>44139.0</v>
       </c>
-      <c r="M2" s="79" t="s">
+      <c r="M2" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="N2" s="79" t="s">
-        <v>173</v>
-      </c>
-      <c r="O2" s="82" t="s">
+      <c r="N2" s="80" t="s">
+        <v>174</v>
+      </c>
+      <c r="O2" s="83" t="s">
         <v>27</v>
       </c>
       <c r="P2" s="28"/>
@@ -10993,13 +11010,13 @@
     </row>
     <row r="3">
       <c r="A3" s="13" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>17</v>
@@ -11013,7 +11030,7 @@
       <c r="K3" s="14"/>
       <c r="L3" s="14"/>
       <c r="M3" s="13" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="N3" s="13" t="s">
         <v>20</v>
@@ -11035,13 +11052,13 @@
     </row>
     <row r="4">
       <c r="A4" s="13" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>25</v>
@@ -11050,7 +11067,7 @@
         <v>17</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G4" s="14"/>
       <c r="H4" s="14"/>
@@ -11064,10 +11081,10 @@
         <v>19</v>
       </c>
       <c r="N4" s="13" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="O4" s="45" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="P4" s="14"/>
       <c r="Q4" s="14"/>
@@ -11134,7 +11151,7 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="90" t="s">
+      <c r="C1" s="93" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -11175,58 +11192,62 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="60" t="s">
-        <v>251</v>
-      </c>
-      <c r="B2" s="60" t="s">
+      <c r="A2" s="94" t="s">
         <v>252</v>
       </c>
-      <c r="C2" s="91" t="s">
+      <c r="B2" s="95" t="s">
         <v>253</v>
       </c>
-      <c r="D2" s="92" t="s">
+      <c r="C2" s="96" t="s">
         <v>254</v>
       </c>
-      <c r="E2" s="93" t="s">
+      <c r="D2" s="97" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="97" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="60" t="s">
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="97" t="s">
         <v>255</v>
       </c>
-      <c r="J2" s="94" t="s">
+      <c r="J2" s="99" t="s">
         <v>256</v>
       </c>
-      <c r="K2" s="81">
+      <c r="K2" s="100">
         <v>43560.0</v>
       </c>
-      <c r="L2" s="81">
+      <c r="L2" s="100">
         <v>44139.0</v>
       </c>
-      <c r="M2" s="60" t="s">
+      <c r="M2" s="97" t="s">
         <v>19</v>
       </c>
-      <c r="N2" s="95" t="s">
-        <v>109</v>
-      </c>
-      <c r="O2" s="96" t="s">
+      <c r="N2" s="97" t="s">
+        <v>110</v>
+      </c>
+      <c r="O2" s="101" t="s">
         <v>27</v>
       </c>
-      <c r="P2" s="28"/>
-      <c r="Q2" s="28"/>
-      <c r="R2" s="23"/>
-      <c r="S2" s="23"/>
-      <c r="T2" s="23"/>
-      <c r="U2" s="23"/>
-      <c r="V2" s="23"/>
-      <c r="W2" s="23"/>
-      <c r="X2" s="23"/>
-      <c r="Y2" s="23"/>
-      <c r="Z2" s="23"/>
-      <c r="AA2" s="23"/>
-      <c r="AB2" s="23"/>
+      <c r="P2" s="98"/>
+      <c r="Q2" s="98"/>
+      <c r="R2" s="98"/>
+      <c r="S2" s="98"/>
+      <c r="T2" s="98"/>
+      <c r="U2" s="98"/>
+      <c r="V2" s="98"/>
+      <c r="W2" s="98"/>
+      <c r="X2" s="98"/>
+      <c r="Y2" s="98"/>
+      <c r="Z2" s="98"/>
+      <c r="AA2" s="98"/>
+      <c r="AB2" s="98"/>
+      <c r="AC2" s="98"/>
+      <c r="AD2" s="98"/>
+      <c r="AE2" s="98"/>
+      <c r="AF2" s="98"/>
     </row>
     <row r="3">
       <c r="A3" s="59" t="s">
@@ -11245,14 +11266,14 @@
       <c r="F3" s="23"/>
       <c r="G3" s="23"/>
       <c r="H3" s="23"/>
-      <c r="I3" s="97" t="s">
+      <c r="I3" s="102" t="s">
         <v>260</v>
       </c>
       <c r="J3" s="23"/>
       <c r="K3" s="25">
         <v>44160.0</v>
       </c>
-      <c r="L3" s="98">
+      <c r="L3" s="103">
         <v>44734.0</v>
       </c>
       <c r="M3" s="62" t="s">
@@ -11261,8 +11282,8 @@
       <c r="N3" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="O3" s="97" t="s">
-        <v>121</v>
+      <c r="O3" s="102" t="s">
+        <v>122</v>
       </c>
       <c r="P3" s="28"/>
       <c r="Q3" s="28"/>
@@ -11277,6 +11298,10 @@
       <c r="Z3" s="23"/>
       <c r="AA3" s="23"/>
       <c r="AB3" s="23"/>
+      <c r="AC3" s="23"/>
+      <c r="AD3" s="23"/>
+      <c r="AE3" s="23"/>
+      <c r="AF3" s="23"/>
     </row>
     <row r="4">
       <c r="A4" s="13" t="s">
@@ -11323,6 +11348,10 @@
       <c r="Z4" s="14"/>
       <c r="AA4" s="14"/>
       <c r="AB4" s="14"/>
+      <c r="AC4" s="14"/>
+      <c r="AD4" s="14"/>
+      <c r="AE4" s="14"/>
+      <c r="AF4" s="14"/>
     </row>
     <row r="5">
       <c r="A5" s="59" t="s">
@@ -11341,7 +11370,7 @@
       <c r="F5" s="23"/>
       <c r="G5" s="23"/>
       <c r="H5" s="23"/>
-      <c r="I5" s="99" t="s">
+      <c r="I5" s="104" t="s">
         <v>268</v>
       </c>
       <c r="J5" s="59"/>
@@ -11353,9 +11382,9 @@
         <v>19</v>
       </c>
       <c r="N5" s="59" t="s">
-        <v>79</v>
-      </c>
-      <c r="O5" s="97" t="s">
+        <v>80</v>
+      </c>
+      <c r="O5" s="102" t="s">
         <v>37</v>
       </c>
       <c r="P5" s="28"/>
@@ -11371,6 +11400,10 @@
       <c r="Z5" s="23"/>
       <c r="AA5" s="23"/>
       <c r="AB5" s="23"/>
+      <c r="AC5" s="23"/>
+      <c r="AD5" s="23"/>
+      <c r="AE5" s="23"/>
+      <c r="AF5" s="23"/>
     </row>
     <row r="6">
       <c r="A6" s="13" t="s">
@@ -11417,6 +11450,10 @@
       <c r="Z6" s="14"/>
       <c r="AA6" s="14"/>
       <c r="AB6" s="14"/>
+      <c r="AC6" s="14"/>
+      <c r="AD6" s="14"/>
+      <c r="AE6" s="14"/>
+      <c r="AF6" s="14"/>
     </row>
     <row r="7">
       <c r="A7" s="13" t="s">
@@ -11463,6 +11500,10 @@
       <c r="Z7" s="14"/>
       <c r="AA7" s="14"/>
       <c r="AB7" s="14"/>
+      <c r="AC7" s="14"/>
+      <c r="AD7" s="14"/>
+      <c r="AE7" s="14"/>
+      <c r="AF7" s="14"/>
     </row>
     <row r="8">
       <c r="A8" s="13" t="s">
@@ -11509,6 +11550,10 @@
       <c r="Z8" s="14"/>
       <c r="AA8" s="14"/>
       <c r="AB8" s="14"/>
+      <c r="AC8" s="14"/>
+      <c r="AD8" s="14"/>
+      <c r="AE8" s="14"/>
+      <c r="AF8" s="14"/>
     </row>
     <row r="9">
       <c r="A9" s="13" t="s">
@@ -11555,6 +11600,10 @@
       <c r="Z9" s="14"/>
       <c r="AA9" s="14"/>
       <c r="AB9" s="14"/>
+      <c r="AC9" s="14"/>
+      <c r="AD9" s="14"/>
+      <c r="AE9" s="14"/>
+      <c r="AF9" s="14"/>
     </row>
     <row r="10">
       <c r="A10" s="13" t="s">
@@ -11601,6 +11650,10 @@
       <c r="Z10" s="14"/>
       <c r="AA10" s="14"/>
       <c r="AB10" s="14"/>
+      <c r="AC10" s="14"/>
+      <c r="AD10" s="14"/>
+      <c r="AE10" s="14"/>
+      <c r="AF10" s="14"/>
     </row>
     <row r="11">
       <c r="A11" s="13" t="s">
@@ -11647,6 +11700,10 @@
       <c r="Z11" s="14"/>
       <c r="AA11" s="14"/>
       <c r="AB11" s="14"/>
+      <c r="AC11" s="14"/>
+      <c r="AD11" s="14"/>
+      <c r="AE11" s="14"/>
+      <c r="AF11" s="14"/>
     </row>
     <row r="12">
       <c r="A12" s="13" t="s">
@@ -11693,6 +11750,10 @@
       <c r="Z12" s="14"/>
       <c r="AA12" s="14"/>
       <c r="AB12" s="14"/>
+      <c r="AC12" s="14"/>
+      <c r="AD12" s="14"/>
+      <c r="AE12" s="14"/>
+      <c r="AF12" s="14"/>
     </row>
     <row r="13">
       <c r="A13" s="13" t="s">
@@ -11741,6 +11802,10 @@
       <c r="Z13" s="14"/>
       <c r="AA13" s="14"/>
       <c r="AB13" s="14"/>
+      <c r="AC13" s="14"/>
+      <c r="AD13" s="14"/>
+      <c r="AE13" s="14"/>
+      <c r="AF13" s="14"/>
     </row>
     <row r="14">
       <c r="A14" s="13" t="s">
@@ -11787,6 +11852,10 @@
       <c r="Z14" s="14"/>
       <c r="AA14" s="14"/>
       <c r="AB14" s="14"/>
+      <c r="AC14" s="14"/>
+      <c r="AD14" s="14"/>
+      <c r="AE14" s="14"/>
+      <c r="AF14" s="14"/>
     </row>
     <row r="15">
       <c r="A15" s="13" t="s">
@@ -11833,6 +11902,10 @@
       <c r="Z15" s="14"/>
       <c r="AA15" s="14"/>
       <c r="AB15" s="14"/>
+      <c r="AC15" s="14"/>
+      <c r="AD15" s="14"/>
+      <c r="AE15" s="14"/>
+      <c r="AF15" s="14"/>
     </row>
     <row r="16">
       <c r="A16" s="13" t="s">
@@ -11879,6 +11952,10 @@
       <c r="Z16" s="14"/>
       <c r="AA16" s="14"/>
       <c r="AB16" s="14"/>
+      <c r="AC16" s="14"/>
+      <c r="AD16" s="14"/>
+      <c r="AE16" s="14"/>
+      <c r="AF16" s="14"/>
     </row>
     <row r="17">
       <c r="A17" s="13" t="s">
@@ -11925,6 +12002,10 @@
       <c r="Z17" s="14"/>
       <c r="AA17" s="14"/>
       <c r="AB17" s="14"/>
+      <c r="AC17" s="14"/>
+      <c r="AD17" s="14"/>
+      <c r="AE17" s="14"/>
+      <c r="AF17" s="14"/>
     </row>
     <row r="18">
       <c r="A18" s="13" t="s">
@@ -11971,6 +12052,10 @@
       <c r="Z18" s="14"/>
       <c r="AA18" s="14"/>
       <c r="AB18" s="14"/>
+      <c r="AC18" s="14"/>
+      <c r="AD18" s="14"/>
+      <c r="AE18" s="14"/>
+      <c r="AF18" s="14"/>
     </row>
     <row r="19">
       <c r="A19" s="13" t="s">
@@ -12017,6 +12102,10 @@
       <c r="Z19" s="14"/>
       <c r="AA19" s="14"/>
       <c r="AB19" s="14"/>
+      <c r="AC19" s="14"/>
+      <c r="AD19" s="14"/>
+      <c r="AE19" s="14"/>
+      <c r="AF19" s="14"/>
     </row>
     <row r="20">
       <c r="A20" s="13" t="s">
@@ -12065,6 +12154,10 @@
       <c r="Z20" s="14"/>
       <c r="AA20" s="14"/>
       <c r="AB20" s="14"/>
+      <c r="AC20" s="14"/>
+      <c r="AD20" s="14"/>
+      <c r="AE20" s="14"/>
+      <c r="AF20" s="14"/>
     </row>
     <row r="21">
       <c r="A21" s="13" t="s">
@@ -12113,6 +12206,10 @@
       <c r="Z21" s="14"/>
       <c r="AA21" s="14"/>
       <c r="AB21" s="14"/>
+      <c r="AC21" s="14"/>
+      <c r="AD21" s="14"/>
+      <c r="AE21" s="14"/>
+      <c r="AF21" s="14"/>
     </row>
     <row r="22">
       <c r="A22" s="13" t="s">
@@ -12159,6 +12256,10 @@
       <c r="Z22" s="14"/>
       <c r="AA22" s="14"/>
       <c r="AB22" s="14"/>
+      <c r="AC22" s="14"/>
+      <c r="AD22" s="14"/>
+      <c r="AE22" s="14"/>
+      <c r="AF22" s="14"/>
     </row>
     <row r="23">
       <c r="A23" s="13" t="s">
@@ -12207,6 +12308,10 @@
       <c r="Z23" s="14"/>
       <c r="AA23" s="14"/>
       <c r="AB23" s="14"/>
+      <c r="AC23" s="14"/>
+      <c r="AD23" s="14"/>
+      <c r="AE23" s="14"/>
+      <c r="AF23" s="14"/>
     </row>
     <row r="24">
       <c r="A24" s="13" t="s">
@@ -12255,6 +12360,10 @@
       <c r="Z24" s="14"/>
       <c r="AA24" s="14"/>
       <c r="AB24" s="14"/>
+      <c r="AC24" s="14"/>
+      <c r="AD24" s="14"/>
+      <c r="AE24" s="14"/>
+      <c r="AF24" s="14"/>
     </row>
     <row r="25">
       <c r="A25" s="13" t="s">
@@ -12303,6 +12412,10 @@
       <c r="Z25" s="14"/>
       <c r="AA25" s="14"/>
       <c r="AB25" s="14"/>
+      <c r="AC25" s="14"/>
+      <c r="AD25" s="14"/>
+      <c r="AE25" s="14"/>
+      <c r="AF25" s="14"/>
     </row>
     <row r="26">
       <c r="A26" s="13" t="s">
@@ -12349,6 +12462,10 @@
       <c r="Z26" s="14"/>
       <c r="AA26" s="14"/>
       <c r="AB26" s="14"/>
+      <c r="AC26" s="14"/>
+      <c r="AD26" s="14"/>
+      <c r="AE26" s="14"/>
+      <c r="AF26" s="14"/>
     </row>
     <row r="27">
       <c r="A27" s="13" t="s">
@@ -12395,6 +12512,10 @@
       <c r="Z27" s="14"/>
       <c r="AA27" s="14"/>
       <c r="AB27" s="14"/>
+      <c r="AC27" s="14"/>
+      <c r="AD27" s="14"/>
+      <c r="AE27" s="14"/>
+      <c r="AF27" s="14"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A13:B14">
@@ -12407,17 +12528,17 @@
       <formula>$M11="proposed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:AB39">
+  <conditionalFormatting sqref="A2:AF39">
     <cfRule type="expression" dxfId="3" priority="3">
       <formula>$M2="proposed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:AB39">
+  <conditionalFormatting sqref="A2:AF39">
     <cfRule type="expression" dxfId="2" priority="4">
       <formula>$M2="accepted"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:AB39">
+  <conditionalFormatting sqref="A2:AF39">
     <cfRule type="expression" dxfId="0" priority="5">
       <formula>$M2="changed"</formula>
     </cfRule>

</xml_diff>